<commit_message>
2022-10-25 - Corrected FEC_IDs
</commit_message>
<xml_diff>
--- a/Data/2022 Candidates File/party_ind_data.xlsx
+++ b/Data/2022 Candidates File/party_ind_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onest\OneDrive\Desktop\2022 Election Model\Data\2022 Candidates File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF62C8A-944A-4DEB-94B1-39726E1C698C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{335CE5A9-988E-4069-BAA8-D1420BB4BFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="290" yWindow="4950" windowWidth="16920" windowHeight="10450" xr2:uid="{EBDE48A5-2C6B-4379-BD39-1564C1B4D6E6}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="party_ind_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="58">
   <si>
     <t>year</t>
   </si>
@@ -212,8 +199,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,16 +208,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -238,15 +525,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -557,13 +1033,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84464BEB-B617-4CE3-ACE5-0300B2F036F6}">
-  <dimension ref="A1:H435"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H436"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A436" sqref="A436"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -8294,16 +8767,16 @@
         <v>2022</v>
       </c>
       <c r="B298" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C298">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D298">
         <v>1</v>
       </c>
       <c r="E298">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F298">
         <v>0</v>
@@ -8312,7 +8785,7 @@
         <v>0</v>
       </c>
       <c r="H298">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.35">
@@ -8320,7 +8793,7 @@
         <v>2022</v>
       </c>
       <c r="B299" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -8329,7 +8802,7 @@
         <v>1</v>
       </c>
       <c r="E299">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F299">
         <v>0</v>
@@ -8338,7 +8811,7 @@
         <v>0</v>
       </c>
       <c r="H299">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.35">
@@ -8349,7 +8822,7 @@
         <v>42</v>
       </c>
       <c r="C300">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D300">
         <v>1</v>
@@ -8375,7 +8848,7 @@
         <v>42</v>
       </c>
       <c r="C301">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -8401,7 +8874,7 @@
         <v>42</v>
       </c>
       <c r="C302">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D302">
         <v>1</v>
@@ -8427,7 +8900,7 @@
         <v>42</v>
       </c>
       <c r="C303">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D303">
         <v>1</v>
@@ -8453,7 +8926,7 @@
         <v>42</v>
       </c>
       <c r="C304">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D304">
         <v>1</v>
@@ -8479,7 +8952,7 @@
         <v>42</v>
       </c>
       <c r="C305">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -8505,7 +8978,7 @@
         <v>42</v>
       </c>
       <c r="C306">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D306">
         <v>1</v>
@@ -8531,7 +9004,7 @@
         <v>42</v>
       </c>
       <c r="C307">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -8557,7 +9030,7 @@
         <v>42</v>
       </c>
       <c r="C308">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D308">
         <v>1</v>
@@ -8583,7 +9056,7 @@
         <v>42</v>
       </c>
       <c r="C309">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D309">
         <v>1</v>
@@ -8609,7 +9082,7 @@
         <v>42</v>
       </c>
       <c r="C310">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -8635,7 +9108,7 @@
         <v>42</v>
       </c>
       <c r="C311">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D311">
         <v>1</v>
@@ -8661,7 +9134,7 @@
         <v>42</v>
       </c>
       <c r="C312">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -8687,7 +9160,7 @@
         <v>42</v>
       </c>
       <c r="C313">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D313">
         <v>1</v>
@@ -8710,10 +9183,10 @@
         <v>2022</v>
       </c>
       <c r="B314" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C314">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D314">
         <v>1</v>
@@ -8728,7 +9201,7 @@
         <v>0</v>
       </c>
       <c r="H314">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.35">
@@ -8739,7 +9212,7 @@
         <v>43</v>
       </c>
       <c r="C315">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D315">
         <v>1</v>
@@ -8765,7 +9238,7 @@
         <v>43</v>
       </c>
       <c r="C316">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D316">
         <v>1</v>
@@ -8780,7 +9253,7 @@
         <v>0</v>
       </c>
       <c r="H316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.35">
@@ -8791,7 +9264,7 @@
         <v>43</v>
       </c>
       <c r="C317">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -8817,7 +9290,7 @@
         <v>43</v>
       </c>
       <c r="C318">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D318">
         <v>1</v>
@@ -8832,7 +9305,7 @@
         <v>0</v>
       </c>
       <c r="H318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.35">
@@ -8840,10 +9313,10 @@
         <v>2022</v>
       </c>
       <c r="B319" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C319">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D319">
         <v>1</v>
@@ -8858,7 +9331,7 @@
         <v>0</v>
       </c>
       <c r="H319">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.35">
@@ -8869,7 +9342,7 @@
         <v>44</v>
       </c>
       <c r="C320">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -8895,7 +9368,7 @@
         <v>44</v>
       </c>
       <c r="C321">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -8910,7 +9383,7 @@
         <v>0</v>
       </c>
       <c r="H321">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.35">
@@ -8921,7 +9394,7 @@
         <v>44</v>
       </c>
       <c r="C322">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -8930,7 +9403,7 @@
         <v>1</v>
       </c>
       <c r="F322">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G322">
         <v>0</v>
@@ -8947,7 +9420,7 @@
         <v>44</v>
       </c>
       <c r="C323">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -8956,13 +9429,13 @@
         <v>1</v>
       </c>
       <c r="F323">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G323">
         <v>0</v>
       </c>
       <c r="H323">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.35">
@@ -8973,7 +9446,7 @@
         <v>44</v>
       </c>
       <c r="C324">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D324">
         <v>1</v>
@@ -8996,10 +9469,10 @@
         <v>2022</v>
       </c>
       <c r="B325" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C325">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D325">
         <v>1</v>
@@ -9025,7 +9498,7 @@
         <v>45</v>
       </c>
       <c r="C326">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -9051,10 +9524,10 @@
         <v>45</v>
       </c>
       <c r="C327">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D327">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E327">
         <v>1</v>
@@ -9077,10 +9550,10 @@
         <v>45</v>
       </c>
       <c r="C328">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E328">
         <v>1</v>
@@ -9103,7 +9576,7 @@
         <v>45</v>
       </c>
       <c r="C329">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D329">
         <v>1</v>
@@ -9129,7 +9602,7 @@
         <v>45</v>
       </c>
       <c r="C330">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D330">
         <v>1</v>
@@ -9155,7 +9628,7 @@
         <v>45</v>
       </c>
       <c r="C331">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D331">
         <v>1</v>
@@ -9181,7 +9654,7 @@
         <v>45</v>
       </c>
       <c r="C332">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D332">
         <v>1</v>
@@ -9207,7 +9680,7 @@
         <v>45</v>
       </c>
       <c r="C333">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D333">
         <v>1</v>
@@ -9233,7 +9706,7 @@
         <v>45</v>
       </c>
       <c r="C334">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D334">
         <v>1</v>
@@ -9259,7 +9732,7 @@
         <v>45</v>
       </c>
       <c r="C335">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D335">
         <v>1</v>
@@ -9285,7 +9758,7 @@
         <v>45</v>
       </c>
       <c r="C336">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D336">
         <v>1</v>
@@ -9311,13 +9784,13 @@
         <v>45</v>
       </c>
       <c r="C337">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D337">
         <v>1</v>
       </c>
       <c r="E337">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F337">
         <v>0</v>
@@ -9337,7 +9810,7 @@
         <v>45</v>
       </c>
       <c r="C338">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D338">
         <v>1</v>
@@ -9363,13 +9836,13 @@
         <v>45</v>
       </c>
       <c r="C339">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D339">
         <v>1</v>
       </c>
       <c r="E339">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F339">
         <v>0</v>
@@ -9389,7 +9862,7 @@
         <v>45</v>
       </c>
       <c r="C340">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D340">
         <v>1</v>
@@ -9415,7 +9888,7 @@
         <v>45</v>
       </c>
       <c r="C341">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D341">
         <v>1</v>
@@ -9438,10 +9911,10 @@
         <v>2022</v>
       </c>
       <c r="B342" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C342">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D342">
         <v>1</v>
@@ -9467,7 +9940,7 @@
         <v>46</v>
       </c>
       <c r="C343">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D343">
         <v>1</v>
@@ -9490,10 +9963,10 @@
         <v>2022</v>
       </c>
       <c r="B344" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C344">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D344">
         <v>1</v>
@@ -9519,7 +9992,7 @@
         <v>47</v>
       </c>
       <c r="C345">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D345">
         <v>1</v>
@@ -9545,13 +10018,13 @@
         <v>47</v>
       </c>
       <c r="C346">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D346">
         <v>1</v>
       </c>
       <c r="E346">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F346">
         <v>0</v>
@@ -9571,7 +10044,7 @@
         <v>47</v>
       </c>
       <c r="C347">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D347">
         <v>1</v>
@@ -9597,19 +10070,19 @@
         <v>47</v>
       </c>
       <c r="C348">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D348">
         <v>1</v>
       </c>
       <c r="E348">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F348">
         <v>0</v>
       </c>
       <c r="G348">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H348">
         <v>0</v>
@@ -9623,7 +10096,7 @@
         <v>47</v>
       </c>
       <c r="C349">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D349">
         <v>1</v>
@@ -9635,7 +10108,7 @@
         <v>0</v>
       </c>
       <c r="G349">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H349">
         <v>0</v>
@@ -9649,7 +10122,7 @@
         <v>47</v>
       </c>
       <c r="C350">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D350">
         <v>1</v>
@@ -9672,19 +10145,19 @@
         <v>2022</v>
       </c>
       <c r="B351" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C351">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D351">
         <v>1</v>
       </c>
       <c r="E351">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F351">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9698,7 +10171,7 @@
         <v>2022</v>
       </c>
       <c r="B352" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C352">
         <v>1</v>
@@ -9707,16 +10180,16 @@
         <v>1</v>
       </c>
       <c r="E352">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F352">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G352">
         <v>0</v>
       </c>
       <c r="H352">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.35">
@@ -9727,7 +10200,7 @@
         <v>49</v>
       </c>
       <c r="C353">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D353">
         <v>1</v>
@@ -9742,7 +10215,7 @@
         <v>0</v>
       </c>
       <c r="H353">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.35">
@@ -9753,7 +10226,7 @@
         <v>49</v>
       </c>
       <c r="C354">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D354">
         <v>1</v>
@@ -9768,7 +10241,7 @@
         <v>0</v>
       </c>
       <c r="H354">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.35">
@@ -9779,7 +10252,7 @@
         <v>49</v>
       </c>
       <c r="C355">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D355">
         <v>1</v>
@@ -9805,7 +10278,7 @@
         <v>49</v>
       </c>
       <c r="C356">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D356">
         <v>1</v>
@@ -9831,7 +10304,7 @@
         <v>49</v>
       </c>
       <c r="C357">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D357">
         <v>1</v>
@@ -9846,7 +10319,7 @@
         <v>0</v>
       </c>
       <c r="H357">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358" spans="1:8" x14ac:dyDescent="0.35">
@@ -9857,7 +10330,7 @@
         <v>49</v>
       </c>
       <c r="C358">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D358">
         <v>1</v>
@@ -9872,7 +10345,7 @@
         <v>0</v>
       </c>
       <c r="H358">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.35">
@@ -9883,7 +10356,7 @@
         <v>49</v>
       </c>
       <c r="C359">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D359">
         <v>1</v>
@@ -9909,7 +10382,7 @@
         <v>49</v>
       </c>
       <c r="C360">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D360">
         <v>1</v>
@@ -9932,10 +10405,10 @@
         <v>2022</v>
       </c>
       <c r="B361" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C361">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D361">
         <v>1</v>
@@ -9950,7 +10423,7 @@
         <v>0</v>
       </c>
       <c r="H361">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:8" x14ac:dyDescent="0.35">
@@ -9961,7 +10434,7 @@
         <v>50</v>
       </c>
       <c r="C362">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D362">
         <v>1</v>
@@ -9987,7 +10460,7 @@
         <v>50</v>
       </c>
       <c r="C363">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D363">
         <v>1</v>
@@ -9996,7 +10469,7 @@
         <v>1</v>
       </c>
       <c r="F363">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -10013,7 +10486,7 @@
         <v>50</v>
       </c>
       <c r="C364">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D364">
         <v>1</v>
@@ -10039,7 +10512,7 @@
         <v>50</v>
       </c>
       <c r="C365">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D365">
         <v>1</v>
@@ -10065,16 +10538,16 @@
         <v>50</v>
       </c>
       <c r="C366">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D366">
         <v>1</v>
       </c>
       <c r="E366">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F366">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G366">
         <v>0</v>
@@ -10091,13 +10564,13 @@
         <v>50</v>
       </c>
       <c r="C367">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D367">
         <v>1</v>
       </c>
       <c r="E367">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F367">
         <v>0</v>
@@ -10117,7 +10590,7 @@
         <v>50</v>
       </c>
       <c r="C368">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D368">
         <v>1</v>
@@ -10126,7 +10599,7 @@
         <v>1</v>
       </c>
       <c r="F368">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G368">
         <v>0</v>
@@ -10143,7 +10616,7 @@
         <v>50</v>
       </c>
       <c r="C369">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D369">
         <v>1</v>
@@ -10152,7 +10625,7 @@
         <v>1</v>
       </c>
       <c r="F369">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G369">
         <v>0</v>
@@ -10169,7 +10642,7 @@
         <v>50</v>
       </c>
       <c r="C370">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D370">
         <v>1</v>
@@ -10178,7 +10651,7 @@
         <v>1</v>
       </c>
       <c r="F370">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G370">
         <v>0</v>
@@ -10195,16 +10668,16 @@
         <v>50</v>
       </c>
       <c r="C371">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D371">
         <v>1</v>
       </c>
       <c r="E371">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F371">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -10221,13 +10694,13 @@
         <v>50</v>
       </c>
       <c r="C372">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D372">
         <v>1</v>
       </c>
       <c r="E372">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F372">
         <v>0</v>
@@ -10247,7 +10720,7 @@
         <v>50</v>
       </c>
       <c r="C373">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D373">
         <v>1</v>
@@ -10273,7 +10746,7 @@
         <v>50</v>
       </c>
       <c r="C374">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D374">
         <v>1</v>
@@ -10299,7 +10772,7 @@
         <v>50</v>
       </c>
       <c r="C375">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D375">
         <v>1</v>
@@ -10308,7 +10781,7 @@
         <v>1</v>
       </c>
       <c r="F375">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G375">
         <v>0</v>
@@ -10325,7 +10798,7 @@
         <v>50</v>
       </c>
       <c r="C376">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D376">
         <v>1</v>
@@ -10334,7 +10807,7 @@
         <v>1</v>
       </c>
       <c r="F376">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G376">
         <v>0</v>
@@ -10351,7 +10824,7 @@
         <v>50</v>
       </c>
       <c r="C377">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D377">
         <v>1</v>
@@ -10377,7 +10850,7 @@
         <v>50</v>
       </c>
       <c r="C378">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D378">
         <v>1</v>
@@ -10386,13 +10859,13 @@
         <v>1</v>
       </c>
       <c r="F378">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G378">
         <v>0</v>
       </c>
       <c r="H378">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:8" x14ac:dyDescent="0.35">
@@ -10403,16 +10876,16 @@
         <v>50</v>
       </c>
       <c r="C379">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D379">
         <v>1</v>
       </c>
       <c r="E379">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F379">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G379">
         <v>0</v>
@@ -10429,13 +10902,13 @@
         <v>50</v>
       </c>
       <c r="C380">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D380">
         <v>1</v>
       </c>
       <c r="E380">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F380">
         <v>0</v>
@@ -10444,7 +10917,7 @@
         <v>0</v>
       </c>
       <c r="H380">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:8" x14ac:dyDescent="0.35">
@@ -10455,7 +10928,7 @@
         <v>50</v>
       </c>
       <c r="C381">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D381">
         <v>1</v>
@@ -10481,7 +10954,7 @@
         <v>50</v>
       </c>
       <c r="C382">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D382">
         <v>1</v>
@@ -10490,7 +10963,7 @@
         <v>1</v>
       </c>
       <c r="F382">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G382">
         <v>0</v>
@@ -10507,7 +10980,7 @@
         <v>50</v>
       </c>
       <c r="C383">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D383">
         <v>1</v>
@@ -10516,13 +10989,13 @@
         <v>1</v>
       </c>
       <c r="F383">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G383">
         <v>0</v>
       </c>
       <c r="H383">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384" spans="1:8" x14ac:dyDescent="0.35">
@@ -10533,7 +11006,7 @@
         <v>50</v>
       </c>
       <c r="C384">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D384">
         <v>1</v>
@@ -10548,7 +11021,7 @@
         <v>0</v>
       </c>
       <c r="H384">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="1:8" x14ac:dyDescent="0.35">
@@ -10559,13 +11032,13 @@
         <v>50</v>
       </c>
       <c r="C385">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D385">
         <v>1</v>
       </c>
       <c r="E385">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F385">
         <v>0</v>
@@ -10585,7 +11058,7 @@
         <v>50</v>
       </c>
       <c r="C386">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D386">
         <v>1</v>
@@ -10594,7 +11067,7 @@
         <v>0</v>
       </c>
       <c r="F386">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -10611,16 +11084,16 @@
         <v>50</v>
       </c>
       <c r="C387">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D387">
         <v>1</v>
       </c>
       <c r="E387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F387">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G387">
         <v>0</v>
@@ -10637,7 +11110,7 @@
         <v>50</v>
       </c>
       <c r="C388">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D388">
         <v>1</v>
@@ -10663,7 +11136,7 @@
         <v>50</v>
       </c>
       <c r="C389">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D389">
         <v>1</v>
@@ -10689,7 +11162,7 @@
         <v>50</v>
       </c>
       <c r="C390">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D390">
         <v>1</v>
@@ -10698,13 +11171,13 @@
         <v>1</v>
       </c>
       <c r="F390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G390">
         <v>0</v>
       </c>
       <c r="H390">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:8" x14ac:dyDescent="0.35">
@@ -10715,22 +11188,22 @@
         <v>50</v>
       </c>
       <c r="C391">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D391">
         <v>1</v>
       </c>
       <c r="E391">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F391">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G391">
         <v>0</v>
       </c>
       <c r="H391">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392" spans="1:8" x14ac:dyDescent="0.35">
@@ -10741,13 +11214,13 @@
         <v>50</v>
       </c>
       <c r="C392">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D392">
         <v>1</v>
       </c>
       <c r="E392">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F392">
         <v>0</v>
@@ -10767,7 +11240,7 @@
         <v>50</v>
       </c>
       <c r="C393">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D393">
         <v>1</v>
@@ -10776,7 +11249,7 @@
         <v>1</v>
       </c>
       <c r="F393">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G393">
         <v>0</v>
@@ -10793,7 +11266,7 @@
         <v>50</v>
       </c>
       <c r="C394">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D394">
         <v>1</v>
@@ -10802,13 +11275,13 @@
         <v>1</v>
       </c>
       <c r="F394">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G394">
         <v>0</v>
       </c>
       <c r="H394">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395" spans="1:8" x14ac:dyDescent="0.35">
@@ -10819,7 +11292,7 @@
         <v>50</v>
       </c>
       <c r="C395">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D395">
         <v>1</v>
@@ -10834,7 +11307,7 @@
         <v>0</v>
       </c>
       <c r="H395">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396" spans="1:8" x14ac:dyDescent="0.35">
@@ -10845,7 +11318,7 @@
         <v>50</v>
       </c>
       <c r="C396">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D396">
         <v>1</v>
@@ -10871,7 +11344,7 @@
         <v>50</v>
       </c>
       <c r="C397">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D397">
         <v>1</v>
@@ -10880,7 +11353,7 @@
         <v>1</v>
       </c>
       <c r="F397">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G397">
         <v>0</v>
@@ -10897,7 +11370,7 @@
         <v>50</v>
       </c>
       <c r="C398">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D398">
         <v>1</v>
@@ -10906,13 +11379,13 @@
         <v>1</v>
       </c>
       <c r="F398">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G398">
         <v>0</v>
       </c>
       <c r="H398">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.35">
@@ -10920,10 +11393,10 @@
         <v>2022</v>
       </c>
       <c r="B399" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C399">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D399">
         <v>1</v>
@@ -10938,7 +11411,7 @@
         <v>0</v>
       </c>
       <c r="H399">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.35">
@@ -10949,7 +11422,7 @@
         <v>51</v>
       </c>
       <c r="C400">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D400">
         <v>1</v>
@@ -10975,7 +11448,7 @@
         <v>51</v>
       </c>
       <c r="C401">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D401">
         <v>1</v>
@@ -10984,7 +11457,7 @@
         <v>1</v>
       </c>
       <c r="F401">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G401">
         <v>0</v>
@@ -11001,7 +11474,7 @@
         <v>51</v>
       </c>
       <c r="C402">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D402">
         <v>1</v>
@@ -11010,7 +11483,7 @@
         <v>1</v>
       </c>
       <c r="F402">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -11024,10 +11497,10 @@
         <v>2022</v>
       </c>
       <c r="B403" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C403">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D403">
         <v>1</v>
@@ -11036,13 +11509,13 @@
         <v>1</v>
       </c>
       <c r="F403">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G403">
         <v>0</v>
       </c>
       <c r="H403">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.35">
@@ -11050,7 +11523,7 @@
         <v>2022</v>
       </c>
       <c r="B404" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -11062,7 +11535,7 @@
         <v>1</v>
       </c>
       <c r="F404">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -11079,7 +11552,7 @@
         <v>53</v>
       </c>
       <c r="C405">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D405">
         <v>1</v>
@@ -11094,7 +11567,7 @@
         <v>0</v>
       </c>
       <c r="H405">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.35">
@@ -11105,7 +11578,7 @@
         <v>53</v>
       </c>
       <c r="C406">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D406">
         <v>1</v>
@@ -11131,7 +11604,7 @@
         <v>53</v>
       </c>
       <c r="C407">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D407">
         <v>1</v>
@@ -11157,7 +11630,7 @@
         <v>53</v>
       </c>
       <c r="C408">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D408">
         <v>1</v>
@@ -11183,7 +11656,7 @@
         <v>53</v>
       </c>
       <c r="C409">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D409">
         <v>1</v>
@@ -11209,7 +11682,7 @@
         <v>53</v>
       </c>
       <c r="C410">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D410">
         <v>1</v>
@@ -11235,7 +11708,7 @@
         <v>53</v>
       </c>
       <c r="C411">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D411">
         <v>1</v>
@@ -11250,7 +11723,7 @@
         <v>0</v>
       </c>
       <c r="H411">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.35">
@@ -11261,7 +11734,7 @@
         <v>53</v>
       </c>
       <c r="C412">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D412">
         <v>1</v>
@@ -11276,7 +11749,7 @@
         <v>0</v>
       </c>
       <c r="H412">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="413" spans="1:8" x14ac:dyDescent="0.35">
@@ -11287,7 +11760,7 @@
         <v>53</v>
       </c>
       <c r="C413">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D413">
         <v>1</v>
@@ -11313,7 +11786,7 @@
         <v>53</v>
       </c>
       <c r="C414">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D414">
         <v>1</v>
@@ -11336,10 +11809,10 @@
         <v>2022</v>
       </c>
       <c r="B415" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C415">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D415">
         <v>1</v>
@@ -11365,7 +11838,7 @@
         <v>54</v>
       </c>
       <c r="C416">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D416">
         <v>1</v>
@@ -11391,7 +11864,7 @@
         <v>54</v>
       </c>
       <c r="C417">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D417">
         <v>1</v>
@@ -11417,7 +11890,7 @@
         <v>54</v>
       </c>
       <c r="C418">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D418">
         <v>1</v>
@@ -11443,7 +11916,7 @@
         <v>54</v>
       </c>
       <c r="C419">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D419">
         <v>1</v>
@@ -11469,7 +11942,7 @@
         <v>54</v>
       </c>
       <c r="C420">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D420">
         <v>1</v>
@@ -11495,7 +11968,7 @@
         <v>54</v>
       </c>
       <c r="C421">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D421">
         <v>1</v>
@@ -11521,7 +11994,7 @@
         <v>54</v>
       </c>
       <c r="C422">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D422">
         <v>1</v>
@@ -11547,7 +12020,7 @@
         <v>54</v>
       </c>
       <c r="C423">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D423">
         <v>1</v>
@@ -11573,7 +12046,7 @@
         <v>54</v>
       </c>
       <c r="C424">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D424">
         <v>1</v>
@@ -11596,10 +12069,10 @@
         <v>2022</v>
       </c>
       <c r="B425" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C425">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D425">
         <v>1</v>
@@ -11614,7 +12087,7 @@
         <v>0</v>
       </c>
       <c r="H425">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.35">
@@ -11625,7 +12098,7 @@
         <v>55</v>
       </c>
       <c r="C426">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D426">
         <v>1</v>
@@ -11640,7 +12113,7 @@
         <v>0</v>
       </c>
       <c r="H426">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.35">
@@ -11648,10 +12121,10 @@
         <v>2022</v>
       </c>
       <c r="B427" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C427">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D427">
         <v>1</v>
@@ -11677,7 +12150,7 @@
         <v>56</v>
       </c>
       <c r="C428">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D428">
         <v>1</v>
@@ -11692,7 +12165,7 @@
         <v>0</v>
       </c>
       <c r="H428">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="429" spans="1:8" x14ac:dyDescent="0.35">
@@ -11703,7 +12176,7 @@
         <v>56</v>
       </c>
       <c r="C429">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D429">
         <v>1</v>
@@ -11718,7 +12191,7 @@
         <v>0</v>
       </c>
       <c r="H429">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:8" x14ac:dyDescent="0.35">
@@ -11729,7 +12202,7 @@
         <v>56</v>
       </c>
       <c r="C430">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D430">
         <v>1</v>
@@ -11744,7 +12217,7 @@
         <v>0</v>
       </c>
       <c r="H430">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="431" spans="1:8" x14ac:dyDescent="0.35">
@@ -11755,7 +12228,7 @@
         <v>56</v>
       </c>
       <c r="C431">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D431">
         <v>1</v>
@@ -11770,7 +12243,7 @@
         <v>0</v>
       </c>
       <c r="H431">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.35">
@@ -11781,13 +12254,13 @@
         <v>56</v>
       </c>
       <c r="C432">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D432">
         <v>1</v>
       </c>
       <c r="E432">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F432">
         <v>0</v>
@@ -11807,13 +12280,13 @@
         <v>56</v>
       </c>
       <c r="C433">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D433">
         <v>1</v>
       </c>
       <c r="E433">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F433">
         <v>0</v>
@@ -11833,22 +12306,22 @@
         <v>56</v>
       </c>
       <c r="C434">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D434">
         <v>1</v>
       </c>
       <c r="E434">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F434">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G434">
         <v>0</v>
       </c>
       <c r="H434">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.35">
@@ -11856,24 +12329,50 @@
         <v>2022</v>
       </c>
       <c r="B435" t="s">
+        <v>56</v>
+      </c>
+      <c r="C435">
+        <v>8</v>
+      </c>
+      <c r="D435">
+        <v>1</v>
+      </c>
+      <c r="E435">
+        <v>0</v>
+      </c>
+      <c r="F435">
+        <v>1</v>
+      </c>
+      <c r="G435">
+        <v>0</v>
+      </c>
+      <c r="H435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A436">
+        <v>2022</v>
+      </c>
+      <c r="B436" t="s">
         <v>57</v>
       </c>
-      <c r="C435">
-        <v>1</v>
-      </c>
-      <c r="D435">
-        <v>1</v>
-      </c>
-      <c r="E435">
-        <v>1</v>
-      </c>
-      <c r="F435">
-        <v>1</v>
-      </c>
-      <c r="G435">
-        <v>0</v>
-      </c>
-      <c r="H435">
+      <c r="C436">
+        <v>1</v>
+      </c>
+      <c r="D436">
+        <v>1</v>
+      </c>
+      <c r="E436">
+        <v>1</v>
+      </c>
+      <c r="F436">
+        <v>1</v>
+      </c>
+      <c r="G436">
+        <v>0</v>
+      </c>
+      <c r="H436">
         <v>0</v>
       </c>
     </row>

</xml_diff>